<commit_message>
new class added 15th feb
</commit_message>
<xml_diff>
--- a/TestData_Opencart.xlsx
+++ b/TestData_Opencart.xlsx
@@ -114,7 +114,7 @@
     <t>Second review comments First revgfgiew c</t>
   </si>
   <si>
-    <t>t5595577552@test.com</t>
+    <t>t55955778852@test.com</t>
   </si>
 </sst>
 </file>
@@ -497,6 +497,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;8 Sensitivity: Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -505,7 +509,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,5 +600,8 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;8 Sensitivity: Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>